<commit_message>
Update Actividad 1.2 Desarrollo.xlsx
</commit_message>
<xml_diff>
--- a/Actividad 1.2/Actividad 1.2 Desarrollo.xlsx
+++ b/Actividad 1.2/Actividad 1.2 Desarrollo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorio Github\Lab-III---LucasBaez\Actividad 1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F659D7A2-B6D8-475B-9609-C71C429388A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884112AD-C6A6-40BA-9B99-6D05B8C5469A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{04C10C6F-9E4F-4DDD-BB35-FDBE9B234F0A}"/>
+    <workbookView xWindow="20370" yWindow="-1635" windowWidth="29040" windowHeight="15840" xr2:uid="{04C10C6F-9E4F-4DDD-BB35-FDBE9B234F0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -527,62 +527,62 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -779,15 +779,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:colOff>104776</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -801,9 +801,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4810126" y="6638925"/>
-          <a:ext cx="1371599" cy="1314450"/>
+        <a:xfrm flipH="1">
+          <a:off x="4972050" y="6638925"/>
+          <a:ext cx="1228726" cy="1333500"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1134,557 +1134,609 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CA15C2-97A1-4447-9014-7123CB75E795}">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2"/>
-      <c r="I6" s="1" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="10"/>
+      <c r="I6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="10"/>
+      <c r="K6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="2"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="7"/>
-      <c r="I7" s="12" t="s">
+      <c r="F7" s="3"/>
+      <c r="I7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="12" t="s">
+      <c r="J7" s="3"/>
+      <c r="K7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L7" s="8"/>
-      <c r="M7" s="7"/>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="7"/>
-      <c r="I8" s="12" t="s">
+      <c r="F8" s="3"/>
+      <c r="I8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="12" t="s">
+      <c r="J8" s="3"/>
+      <c r="K8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="L8" s="8"/>
-      <c r="M8" s="7"/>
+      <c r="M8" s="3"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="I9" s="12" t="s">
+      <c r="F9" s="3"/>
+      <c r="I9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="12" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L9" s="8"/>
-      <c r="M9" s="7"/>
+      <c r="M9" s="3"/>
     </row>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="7"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
+      <c r="F10" s="3"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="7"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="9" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="11"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="11"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="2"/>
-      <c r="I18" s="1" t="s">
+      <c r="E18" s="11"/>
+      <c r="F18" s="10"/>
+      <c r="I18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="1" t="s">
+      <c r="J18" s="10"/>
+      <c r="K18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="2"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="10"/>
     </row>
     <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="7"/>
-      <c r="I19" s="12" t="s">
+      <c r="F19" s="3"/>
+      <c r="I19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="12" t="s">
+      <c r="J19" s="3"/>
+      <c r="K19" s="7" t="s">
         <v>27</v>
       </c>
       <c r="L19" s="8"/>
-      <c r="M19" s="7"/>
+      <c r="M19" s="3"/>
     </row>
     <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="7"/>
-      <c r="I20" s="12" t="s">
+      <c r="F20" s="3"/>
+      <c r="I20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="12" t="s">
+      <c r="J20" s="3"/>
+      <c r="K20" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L20" s="8"/>
-      <c r="M20" s="7"/>
+      <c r="M20" s="3"/>
     </row>
     <row r="21" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="7"/>
-      <c r="I21" s="12" t="s">
+      <c r="F21" s="3"/>
+      <c r="I21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="12" t="s">
+      <c r="J21" s="3"/>
+      <c r="K21" s="7" t="s">
         <v>30</v>
       </c>
       <c r="L21" s="8"/>
-      <c r="M21" s="7"/>
+      <c r="M21" s="3"/>
     </row>
     <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="8"/>
-      <c r="F22" s="7"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="6"/>
+      <c r="F22" s="3"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="7"/>
+      <c r="M22" s="3"/>
     </row>
     <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="9" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="11"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="6"/>
     </row>
     <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="13"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="11"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="6"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
     </row>
     <row r="28" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H29" s="4"/>
+      <c r="H29" s="20"/>
     </row>
     <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
     </row>
     <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="1" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="2"/>
-      <c r="I31" s="1" t="s">
+      <c r="E31" s="11"/>
+      <c r="F31" s="10"/>
+      <c r="I31" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J31" s="2"/>
-      <c r="K31" s="1" t="s">
+      <c r="J31" s="10"/>
+      <c r="K31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L31" s="5"/>
-      <c r="M31" s="2"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="10"/>
     </row>
     <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="12" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E32" s="8"/>
-      <c r="F32" s="7"/>
-      <c r="I32" s="12" t="s">
+      <c r="F32" s="3"/>
+      <c r="I32" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="17" t="s">
+      <c r="J32" s="3"/>
+      <c r="K32" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="L32" s="18"/>
-      <c r="M32" s="19"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="18"/>
     </row>
     <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="6" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E33" s="8"/>
-      <c r="F33" s="7"/>
-      <c r="I33" s="12" t="s">
+      <c r="F33" s="3"/>
+      <c r="I33" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J33" s="7"/>
-      <c r="K33" s="12" t="s">
+      <c r="J33" s="3"/>
+      <c r="K33" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
-      <c r="N33" s="7"/>
+      <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="6" t="s">
+      <c r="C34" s="3"/>
+      <c r="D34" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="8"/>
-      <c r="F34" s="7"/>
-      <c r="I34" s="12" t="s">
+      <c r="F34" s="3"/>
+      <c r="I34" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J34" s="7"/>
-      <c r="K34" s="12" t="s">
+      <c r="J34" s="3"/>
+      <c r="K34" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="14"/>
     </row>
     <row r="35" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="12" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="7"/>
-      <c r="I35" s="12" t="s">
+      <c r="F35" s="3"/>
+      <c r="I35" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J35" s="7"/>
-      <c r="K35" s="20" t="s">
+      <c r="J35" s="3"/>
+      <c r="K35" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="L35" s="10"/>
-      <c r="M35" s="11"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="6"/>
     </row>
     <row r="36" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="9" t="s">
+      <c r="C36" s="3"/>
+      <c r="D36" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="11"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="11"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="6"/>
     </row>
     <row r="37" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="9" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="11"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="11"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="6"/>
     </row>
     <row r="39" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
     </row>
     <row r="40" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="1" t="s">
+      <c r="G40" s="10"/>
+      <c r="H40" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I40" s="5"/>
-      <c r="J40" s="2"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="10"/>
     </row>
     <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="7"/>
-      <c r="H41" s="12" t="s">
+      <c r="G41" s="3"/>
+      <c r="H41" s="7" t="s">
         <v>54</v>
       </c>
       <c r="I41" s="8"/>
-      <c r="J41" s="7"/>
+      <c r="J41" s="3"/>
     </row>
     <row r="42" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="7"/>
-      <c r="H42" s="12" t="s">
+      <c r="G42" s="3"/>
+      <c r="H42" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I42" s="8"/>
-      <c r="J42" s="7"/>
+      <c r="J42" s="3"/>
     </row>
     <row r="43" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="7"/>
-      <c r="H43" s="12" t="s">
+      <c r="G43" s="3"/>
+      <c r="H43" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I43" s="8"/>
-      <c r="J43" s="7"/>
+      <c r="J43" s="3"/>
     </row>
     <row r="44" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G44" s="7"/>
-      <c r="H44" s="12" t="s">
+      <c r="G44" s="3"/>
+      <c r="H44" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I44" s="8"/>
-      <c r="J44" s="7"/>
+      <c r="J44" s="3"/>
     </row>
     <row r="45" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F45" s="6"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="11"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="6"/>
     </row>
     <row r="46" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F46" s="6"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="11"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="D37:F37"/>
     <mergeCell ref="K33:N33"/>
     <mergeCell ref="I34:J34"/>
@@ -1709,72 +1761,20 @@
     <mergeCell ref="I32:J32"/>
     <mergeCell ref="K32:M32"/>
     <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:J42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>